<commit_message>
Fixed point mass derating. Two track converges in coarse grain
</commit_message>
<xml_diff>
--- a/custom sim/vehicle_files/FEB_SN3_30kW.xlsx
+++ b/custom sim/vehicle_files/FEB_SN3_30kW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Documents\GitHub\FEBSim\custom sim\vehicle_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD83E22-D0EA-4A98-A5D4-763117BA95E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413A916D-680E-44FB-B70B-22E79ED652F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
   <si>
     <t>General</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>with aero, no driver;     245.0</t>
+  </si>
+  <si>
+    <t>Assumed 0.6-0.7 for accuracy</t>
   </si>
 </sst>
 </file>
@@ -2246,8 +2249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2317,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="8">
-        <v>325</v>
+        <v>245</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>6</v>
@@ -2475,7 +2478,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="8">
-        <v>266.7</v>
+        <v>203.2</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>8</v>
@@ -2582,12 +2585,14 @@
         <v>37</v>
       </c>
       <c r="C22" s="8">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="10"/>
+      <c r="E22" s="10" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="36"/>
@@ -2595,7 +2600,7 @@
         <v>31</v>
       </c>
       <c r="C23" s="8">
-        <v>266.7</v>
+        <v>203.2</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>

</xml_diff>